<commit_message>
I started coding three statistical models (Poisson, Horseshoe and Zero-inflated
</commit_message>
<xml_diff>
--- a/data/dataset_neuroscience_1.xlsx
+++ b/data/dataset_neuroscience_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MDASILVA\MDASILVA\ESEO\INTERSHIP\BDA\BDA_Project\BDAJupiterNotebook\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3096CEAE-21FF-4C31-A26F-7C64DA0B0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC635776-1C3A-4921-A936-6E77FE14C49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{C829A673-F44C-49DE-8E9A-B2FC9AA259F4}"/>
+    <workbookView minimized="1" xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="9420" xr2:uid="{C829A673-F44C-49DE-8E9A-B2FC9AA259F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig2_c-Fos counts" sheetId="2" r:id="rId1"/>
@@ -1801,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665CECC1-8FBB-4BDB-A4F2-9DF141040273}">
   <dimension ref="A1:BO52"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12372,7 +12372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D04541A-611B-463C-9C31-3CC317DDD5D3}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>